<commit_message>
update apply DataProviderFactory for practice
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataTest.xlsx
+++ b/src/test/resources/testdata/DataTest.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="addNewCustomer" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>email</t>
   </si>
@@ -52,10 +52,61 @@
     <t>vankhe</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>LTD</t>
+  </si>
+  <si>
+    <t>companyName</t>
+  </si>
+  <si>
+    <t>Viettel</t>
+  </si>
+  <si>
+    <t>vatNumber</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>zipCode</t>
+  </si>
+  <si>
+    <t>HBT</t>
+  </si>
+  <si>
+    <t>667735</t>
+  </si>
+  <si>
+    <t>0852741963</t>
+  </si>
+  <si>
+    <t>hbt.hn.com</t>
+  </si>
+  <si>
+    <t>khoinghia</t>
+  </si>
+  <si>
+    <t>Me Linh</t>
+  </si>
+  <si>
+    <t>Ha Noi</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -521,32 +572,115 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1">
+        <v>28386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>